<commit_message>
changed some comments and responses in q2
</commit_message>
<xml_diff>
--- a/Project3/COMP_421_Team_24_Project_3/Q4/Monthly New Subscriptions.xlsx
+++ b/Project3/COMP_421_Team_24_Project_3/Q4/Monthly New Subscriptions.xlsx
@@ -5,19 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Mystelvric/Documents/Mcgill/Winter 2018/421/Assignment/421DBProject1/Project3/Q4/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Mystelvric/Documents/Mcgill/Winter 2018/421/Assignment/421DBProject1/Project3/COMP_421_Team_24_Project_3/Q4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EE32A1E-6956-E041-A7D3-EEF8F4499358}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3669C6B7-9CA0-3A41-AC71-CF70BE4DCDB5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Monthly New Subscriptions" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -125,7 +122,13 @@
             </a:r>
             <a:r>
               <a:rPr lang="fr-FR" baseline="0"/>
-              <a:t> new subscriptions</a:t>
+              <a:t> new subscriptions </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-FR" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>number</a:t>
             </a:r>
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
@@ -1150,19 +1153,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="plan_prices"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
@@ -1463,7 +1453,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>